<commit_message>
I added the shippment address save functionality in the code
</commit_message>
<xml_diff>
--- a/backend/customer_data.xlsx
+++ b/backend/customer_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -29,21 +29,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>shruti</t>
-  </si>
-  <si>
-    <t>s@gmail.com</t>
-  </si>
-  <si>
-    <t>23 nagri bhopal</t>
-  </si>
-  <si>
-    <t>Bhopal</t>
-  </si>
-  <si>
-    <t>2023-12-14T17:46:04.855Z</t>
   </si>
 </sst>
 </file>
@@ -420,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -464,26 +449,6 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>8433222223</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>